<commit_message>
Updating one gap var only.
</commit_message>
<xml_diff>
--- a/Timed/KFCV_USA_AZ_Pima County_Tucson_Summary.xlsx
+++ b/Timed/KFCV_USA_AZ_Pima County_Tucson_Summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My_software_develops\MobilityPyro\MobilityInference\Timed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DEB4CA7-40CB-481E-8E9D-7908A93A1DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD7C4761-6844-4B57-B9CF-1B91A9FE51E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5545FD4A-4554-4FD8-B599-78E2CFBE2013}"/>
+    <workbookView xWindow="28680" yWindow="-75" windowWidth="29040" windowHeight="15840" xr2:uid="{5545FD4A-4554-4FD8-B599-78E2CFBE2013}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -191,7 +191,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$T$3</c:f>
+              <c:f>Sheet1!$F$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -212,30 +212,30 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$T$4:$T$10</c:f>
+              <c:f>Sheet1!$F$4:$F$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.5724480000000001</c:v>
+                  <c:v>4.8394800000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.4910398</c:v>
+                  <c:v>4.9501656999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5334833000000001</c:v>
+                  <c:v>2.0150065000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.6328020000000001</c:v>
+                  <c:v>3.107965E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.5604724999999999</c:v>
+                  <c:v>2.1879672999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.6534036000000001</c:v>
+                  <c:v>1.3391256000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.7906346</c:v>
+                  <c:v>6.1117887000000003E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -251,7 +251,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$U$3</c:f>
+              <c:f>Sheet1!$G$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -272,30 +272,30 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$U$4:$U$10</c:f>
+              <c:f>Sheet1!$G$4:$G$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.0919859999999999</c:v>
+                  <c:v>0.75264679999999995</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.5938232999999999</c:v>
+                  <c:v>0.1207329</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.6382456000000001</c:v>
+                  <c:v>0.11115849</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.0956209000000001</c:v>
+                  <c:v>0.43173919999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.0323869999999999</c:v>
+                  <c:v>0.4867785</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.6948909999999999</c:v>
+                  <c:v>0.12779294999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.3435606</c:v>
+                  <c:v>0.41818630000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1056,15 +1056,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1389,10 +1389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{523398A0-5BCC-469C-B58B-CDFE67F83BA9}">
-  <dimension ref="A1:U10"/>
+  <dimension ref="A1:U12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+      <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1948,8 +1948,85 @@
         <v>1.3435606</v>
       </c>
     </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <f t="shared" ref="C11" si="0">AVERAGE(C4:C10)</f>
+        <v>2940.8857770647314</v>
+      </c>
+      <c r="E11">
+        <f t="shared" ref="E11:T11" si="1">AVERAGE(E4:E10)</f>
+        <v>4.2899352714285719</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>0.34986216285714283</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="1"/>
+        <v>140822.22167909142</v>
+      </c>
+      <c r="L11">
+        <f t="shared" ref="L11" si="2">AVERAGE(L4:L10)</f>
+        <v>0.43893077285714288</v>
+      </c>
+      <c r="N11">
+        <f t="shared" ref="N11" si="3">AVERAGE(N4:N10)</f>
+        <v>5.3487924714285713</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="1"/>
+        <v>141648.56698343385</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="1"/>
+        <v>0.55249707999999997</v>
+      </c>
+      <c r="U11">
+        <f>AVERAGE(U4:U10)</f>
+        <v>1.6415020571428571</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <f t="shared" ref="B12:D12" si="4">_xlfn.STDEV.P(C4:C10)</f>
+        <v>2026.8518632944815</v>
+      </c>
+      <c r="E12">
+        <f>_xlfn.STDEV.P(E4:E10)</f>
+        <v>1.6605988052455258</v>
+      </c>
+      <c r="G12">
+        <f t="shared" ref="F12:U12" si="5">_xlfn.STDEV.P(G4:G10)</f>
+        <v>0.22397320696090511</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="5"/>
+        <v>22398.321014039695</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="5"/>
+        <v>0.24508297775371748</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="5"/>
+        <v>0.37588288374385115</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="5"/>
+        <v>20900.632733154045</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="5"/>
+        <v>0.20023581383395314</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="5"/>
+        <v>0.32839136463063612</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>